<commit_message>
2022.9.16 update feature selection part
</commit_message>
<xml_diff>
--- a/Supplementary Material/Table S2.xlsx
+++ b/Supplementary Material/Table S2.xlsx
@@ -454,10 +454,10 @@
         <v>0.7887371679440841</v>
       </c>
       <c r="J2">
-        <v>0.800359187184544</v>
+        <v>0.764921615943529</v>
       </c>
       <c r="K2">
-        <v>1.162786252896862</v>
+        <v>1.41579715701792</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -492,10 +492,10 @@
         <v>5.544646073103071</v>
       </c>
       <c r="J3">
-        <v>-0.07863672376673547</v>
+        <v>-0.02778210700594255</v>
       </c>
       <c r="K3">
-        <v>-0.610937995298824</v>
+        <v>-1.250977110889724</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -530,10 +530,10 @@
         <v>-0.06296020057592831</v>
       </c>
       <c r="J4">
-        <v>-0.3706498981603608</v>
+        <v>-0.4121639630965508</v>
       </c>
       <c r="K4">
-        <v>1.063020901347429</v>
+        <v>1.565330006388424</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -568,10 +568,10 @@
         <v>2.319311733646203</v>
       </c>
       <c r="J5">
-        <v>-1.397561645759823</v>
+        <v>-1.404674961225906</v>
       </c>
       <c r="K5">
-        <v>-0.4837015165104872</v>
+        <v>-0.1490900124345091</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -606,10 +606,10 @@
         <v>1.682402994732042</v>
       </c>
       <c r="J6">
-        <v>-1.015622716247039</v>
+        <v>-1.023824340122698</v>
       </c>
       <c r="K6">
-        <v>0.5096753276415469</v>
+        <v>0.4879138760428428</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -644,10 +644,10 @@
         <v>2.703755518156427</v>
       </c>
       <c r="J7">
-        <v>2.779824463322937</v>
+        <v>2.775606969017566</v>
       </c>
       <c r="K7">
-        <v>-1.844987240881946</v>
+        <v>-1.357666680986589</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -682,10 +682,10 @@
         <v>-0.4185890869204154</v>
       </c>
       <c r="J8">
-        <v>2.777492850490418</v>
+        <v>2.688691913548625</v>
       </c>
       <c r="K8">
-        <v>2.3949454100223</v>
+        <v>3.073366636507346</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -720,10 +720,10 @@
         <v>-4.197410244482415</v>
       </c>
       <c r="J9">
-        <v>0.4142655733734634</v>
+        <v>0.4197282583367813</v>
       </c>
       <c r="K9">
-        <v>0.3590015267456111</v>
+        <v>0.05787049749262208</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -758,10 +758,10 @@
         <v>-1.204384498754584</v>
       </c>
       <c r="J10">
-        <v>1.210764878278101</v>
+        <v>1.229979289112443</v>
       </c>
       <c r="K10">
-        <v>-0.5256648826448355</v>
+        <v>-0.8059671170203065</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -796,10 +796,10 @@
         <v>-2.263224377554079</v>
       </c>
       <c r="J11">
-        <v>2.540226004935976</v>
+        <v>2.519145966910474</v>
       </c>
       <c r="K11">
-        <v>0.537384507782815</v>
+        <v>0.7870898601539611</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -834,10 +834,10 @@
         <v>-1.562211833386316</v>
       </c>
       <c r="J12">
-        <v>0.378990163831161</v>
+        <v>0.3899589673706731</v>
       </c>
       <c r="K12">
-        <v>-1.393817540234192</v>
+        <v>-1.19431887500825</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>-2.63302925673281</v>
       </c>
       <c r="J13">
-        <v>1.534067837126955</v>
+        <v>1.612720558057333</v>
       </c>
       <c r="K13">
-        <v>-2.670074170772125</v>
+        <v>-3.130328132858587</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -910,10 +910,10 @@
         <v>-0.6147186649284406</v>
       </c>
       <c r="J14">
-        <v>-1.269828810224148</v>
+        <v>-1.250989408008622</v>
       </c>
       <c r="K14">
-        <v>-1.537002495213574</v>
+        <v>-1.448682946696693</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -948,10 +948,10 @@
         <v>-2.484024609437821</v>
       </c>
       <c r="J15">
-        <v>5.369309456056674</v>
+        <v>5.355162992290753</v>
       </c>
       <c r="K15">
-        <v>0.9855156322985501</v>
+        <v>1.064577411511313</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -986,10 +986,10 @@
         <v>-0.8938780028771925</v>
       </c>
       <c r="J16">
-        <v>3.303961293385418</v>
+        <v>3.231406713876004</v>
       </c>
       <c r="K16">
-        <v>1.345159153572509</v>
+        <v>2.243619496227912</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1024,10 +1024,10 @@
         <v>-3.20605396178474</v>
       </c>
       <c r="J17">
-        <v>3.167633496093954</v>
+        <v>3.201507401183696</v>
       </c>
       <c r="K17">
-        <v>0.2151604915347922</v>
+        <v>-0.3226326671911714</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1062,10 +1062,10 @@
         <v>1.49678836629711</v>
       </c>
       <c r="J18">
-        <v>0.8053587874044872</v>
+        <v>0.8428286439912462</v>
       </c>
       <c r="K18">
-        <v>-2.285075995949182</v>
+        <v>-2.231814506486939</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1100,10 +1100,10 @@
         <v>-0.6781713679681627</v>
       </c>
       <c r="J19">
-        <v>4.759776291797536</v>
+        <v>4.757715666540784</v>
       </c>
       <c r="K19">
-        <v>0.4794223798102067</v>
+        <v>0.3554186571241644</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1138,10 +1138,10 @@
         <v>-0.8062918033034158</v>
       </c>
       <c r="J20">
-        <v>1.028126420023686</v>
+        <v>1.029948223676325</v>
       </c>
       <c r="K20">
-        <v>-1.808676818425582</v>
+        <v>-1.369291647722031</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1176,10 +1176,10 @@
         <v>3.891428612208049</v>
       </c>
       <c r="J21">
-        <v>0.1789620193441996</v>
+        <v>0.1837110069746234</v>
       </c>
       <c r="K21">
-        <v>-1.64106069130296</v>
+        <v>-1.096146192360822</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1214,10 +1214,10 @@
         <v>-2.268066305065672</v>
       </c>
       <c r="J22">
-        <v>-1.112115901829253</v>
+        <v>-1.099246947617361</v>
       </c>
       <c r="K22">
-        <v>0.4739517309458609</v>
+        <v>0.2776068256132322</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1252,10 +1252,10 @@
         <v>-0.1770999679967082</v>
       </c>
       <c r="J23">
-        <v>-1.579490573229064</v>
+        <v>-1.598771731702689</v>
       </c>
       <c r="K23">
-        <v>1.599606193593092</v>
+        <v>1.732984421495257</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -1290,10 +1290,10 @@
         <v>0.8770821758840776</v>
       </c>
       <c r="J24">
-        <v>2.461202693162156</v>
+        <v>2.393968940363753</v>
       </c>
       <c r="K24">
-        <v>3.349977989202716</v>
+        <v>3.699209648823975</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1328,10 +1328,10 @@
         <v>2.725881026995079</v>
       </c>
       <c r="J25">
-        <v>0.05623386186905025</v>
+        <v>0.1289982825288438</v>
       </c>
       <c r="K25">
-        <v>-1.544972865046091</v>
+        <v>-2.097291789190692</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1366,10 +1366,10 @@
         <v>5.480122346437143</v>
       </c>
       <c r="J26">
-        <v>0.7602518790649276</v>
+        <v>0.7728959699828759</v>
       </c>
       <c r="K26">
-        <v>-0.902730759421743</v>
+        <v>-0.965775724362555</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -1404,10 +1404,10 @@
         <v>0.3015484215769767</v>
       </c>
       <c r="J27">
-        <v>-0.1291974293310572</v>
+        <v>-0.1228500114215029</v>
       </c>
       <c r="K27">
-        <v>-0.9163071943539949</v>
+        <v>-0.712991509446211</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -1442,10 +1442,10 @@
         <v>-0.6538660134451413</v>
       </c>
       <c r="J28">
-        <v>0.334672841202834</v>
+        <v>0.2703277798523426</v>
       </c>
       <c r="K28">
-        <v>1.70977244855933</v>
+        <v>2.342945382580352</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1480,10 +1480,10 @@
         <v>0.8976035829847019</v>
       </c>
       <c r="J29">
-        <v>-0.8403569351073669</v>
+        <v>-0.8606524715674024</v>
       </c>
       <c r="K29">
-        <v>-0.06033369567626016</v>
+        <v>0.4031602209989993</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -1518,10 +1518,10 @@
         <v>-4.675644038648593</v>
       </c>
       <c r="J30">
-        <v>-0.09339776901755364</v>
+        <v>-0.04880174717139523</v>
       </c>
       <c r="K30">
-        <v>-0.3953175501163245</v>
+        <v>-0.9864892365242089</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1556,10 +1556,10 @@
         <v>8.049278579242861</v>
       </c>
       <c r="J31">
-        <v>-1.811474131281055</v>
+        <v>-1.7089806616939</v>
       </c>
       <c r="K31">
-        <v>0.2775328056254749</v>
+        <v>-1.696155488963861</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -1594,10 +1594,10 @@
         <v>-2.057224231291881</v>
       </c>
       <c r="J32">
-        <v>-2.575704088791573</v>
+        <v>-2.586885005548173</v>
       </c>
       <c r="K32">
-        <v>1.119375629849191</v>
+        <v>0.9464822754157871</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -1632,10 +1632,10 @@
         <v>-1.504773873342479</v>
       </c>
       <c r="J33">
-        <v>-0.8481891541537103</v>
+        <v>-0.8294435131084817</v>
       </c>
       <c r="K33">
-        <v>-2.004474959747716</v>
+        <v>-1.871665983988318</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -1670,10 +1670,10 @@
         <v>-1.911041683219938</v>
       </c>
       <c r="J34">
-        <v>0.9495336819773521</v>
+        <v>0.8976875158450545</v>
       </c>
       <c r="K34">
-        <v>2.211326101215259</v>
+        <v>2.46292661604369</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -1708,10 +1708,10 @@
         <v>1.905988927530795</v>
       </c>
       <c r="J35">
-        <v>-0.6036342118475968</v>
+        <v>-0.5911711669441005</v>
       </c>
       <c r="K35">
-        <v>-0.5109324228214339</v>
+        <v>-0.5430853638340668</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -1746,10 +1746,10 @@
         <v>-3.980976675296134</v>
       </c>
       <c r="J36">
-        <v>0.8381233267827933</v>
+        <v>0.8810280074469222</v>
       </c>
       <c r="K36">
-        <v>-1.167227841722144</v>
+        <v>-1.495143936553223</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -1784,10 +1784,10 @@
         <v>-1.769935093749309</v>
       </c>
       <c r="J37">
-        <v>0.146483602722687</v>
+        <v>0.2351754816904214</v>
       </c>
       <c r="K37">
-        <v>-1.550301152176966</v>
+        <v>-2.363099184915063</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -1822,10 +1822,10 @@
         <v>-1.689682908465381</v>
       </c>
       <c r="J38">
-        <v>-0.9562494755134338</v>
+        <v>-0.9454557012463654</v>
       </c>
       <c r="K38">
-        <v>-0.6228466748074517</v>
+        <v>-0.7607073610782192</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -1860,10 +1860,10 @@
         <v>2.818137812329879</v>
       </c>
       <c r="J39">
-        <v>0.8346672767972266</v>
+        <v>0.7660045051671217</v>
       </c>
       <c r="K39">
-        <v>1.660777438509934</v>
+        <v>2.300196694345114</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -1898,10 +1898,10 @@
         <v>-0.01792545477251248</v>
       </c>
       <c r="J40">
-        <v>-1.30621265189162</v>
+        <v>-1.298482110086942</v>
       </c>
       <c r="K40">
-        <v>-0.5752615458646776</v>
+        <v>-0.6499506989708825</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -1936,10 +1936,10 @@
         <v>-3.946470182190068</v>
       </c>
       <c r="J41">
-        <v>0.8762027130714053</v>
+        <v>0.8719093992671586</v>
       </c>
       <c r="K41">
-        <v>0.9761982001133632</v>
+        <v>0.8182335381693275</v>
       </c>
       <c r="L41">
         <v>0</v>
@@ -1974,10 +1974,10 @@
         <v>-2.94665405524555</v>
       </c>
       <c r="J42">
-        <v>-0.905972922122224</v>
+        <v>-0.8916665675853146</v>
       </c>
       <c r="K42">
-        <v>-1.417200569100225</v>
+        <v>-1.394874174472765</v>
       </c>
       <c r="L42">
         <v>1</v>
@@ -2012,10 +2012,10 @@
         <v>-2.057809067147165</v>
       </c>
       <c r="J43">
-        <v>0.8638256384739283</v>
+        <v>0.8611138110859424</v>
       </c>
       <c r="K43">
-        <v>-2.689016014277033</v>
+        <v>-1.892600217676562</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -2050,10 +2050,10 @@
         <v>-3.850829109940106</v>
       </c>
       <c r="J44">
-        <v>-1.397953033829993</v>
+        <v>-1.387371642650073</v>
       </c>
       <c r="K44">
-        <v>-2.280546829940794</v>
+        <v>-1.813592189539114</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -2088,10 +2088,10 @@
         <v>-1.609712817651512</v>
       </c>
       <c r="J45">
-        <v>1.699364140912497</v>
+        <v>1.703960368763851</v>
       </c>
       <c r="K45">
-        <v>-1.234364574327157</v>
+        <v>-0.9127956005427429</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -2126,10 +2126,10 @@
         <v>-3.615684084430053</v>
       </c>
       <c r="J46">
-        <v>-1.362435047873008</v>
+        <v>-1.264723014969307</v>
       </c>
       <c r="K46">
-        <v>-0.5130589494696073</v>
+        <v>-1.91604593353955</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -2164,10 +2164,10 @@
         <v>2.954172575095036</v>
       </c>
       <c r="J47">
-        <v>1.571351989895523</v>
+        <v>1.615066843613985</v>
       </c>
       <c r="K47">
-        <v>-1.800706581658395</v>
+        <v>-1.887280320548735</v>
       </c>
       <c r="L47">
         <v>0</v>
@@ -2202,10 +2202,10 @@
         <v>0.8141452712556212</v>
       </c>
       <c r="J48">
-        <v>1.859335860213473</v>
+        <v>1.849302981134918</v>
       </c>
       <c r="K48">
-        <v>0.7177227150499313</v>
+        <v>0.6184832466707841</v>
       </c>
       <c r="L48">
         <v>0</v>
@@ -2240,10 +2240,10 @@
         <v>3.658361879228188</v>
       </c>
       <c r="J49">
-        <v>3.516297192925694</v>
+        <v>3.504041669636051</v>
       </c>
       <c r="K49">
-        <v>0.8075016915515804</v>
+        <v>0.7731565892909081</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -2278,10 +2278,10 @@
         <v>-1.483291453823529</v>
       </c>
       <c r="J50">
-        <v>0.2818698796127943</v>
+        <v>0.321651056598046</v>
       </c>
       <c r="K50">
-        <v>-2.207149223494466</v>
+        <v>-2.340668125325949</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -2316,10 +2316,10 @@
         <v>2.168955711043087</v>
       </c>
       <c r="J51">
-        <v>0.883821436078792</v>
+        <v>0.8648655047661653</v>
       </c>
       <c r="K51">
-        <v>-0.9774679271261079</v>
+        <v>-0.4450984243841053</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -2354,10 +2354,10 @@
         <v>0.8862076883733326</v>
       </c>
       <c r="J52">
-        <v>1.212997860431934</v>
+        <v>1.159336610031126</v>
       </c>
       <c r="K52">
-        <v>-0.6728552542966804</v>
+        <v>0.393320322664216</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -2392,10 +2392,10 @@
         <v>1.467646739375813</v>
       </c>
       <c r="J53">
-        <v>1.173779018942096</v>
+        <v>1.276744879717702</v>
       </c>
       <c r="K53">
-        <v>-0.4607351307006594</v>
+        <v>-1.809548772720315</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -2430,10 +2430,10 @@
         <v>-2.607149497524277</v>
       </c>
       <c r="J54">
-        <v>4.0859035165618</v>
+        <v>4.088558859431215</v>
       </c>
       <c r="K54">
-        <v>2.202200637811937</v>
+        <v>1.688135276470911</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -2468,10 +2468,10 @@
         <v>3.428620010554541</v>
       </c>
       <c r="J55">
-        <v>-2.165712622205415</v>
+        <v>-2.153167188925035</v>
       </c>
       <c r="K55">
-        <v>0.708516433937934</v>
+        <v>0.1711778911504245</v>
       </c>
       <c r="L55">
         <v>1</v>
@@ -2506,10 +2506,10 @@
         <v>-4.006738926551512</v>
       </c>
       <c r="J56">
-        <v>1.019317272247096</v>
+        <v>1.040127398145381</v>
       </c>
       <c r="K56">
-        <v>0.06229962551870375</v>
+        <v>-0.1938909221915296</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -2544,10 +2544,10 @@
         <v>1.906272033505535</v>
       </c>
       <c r="J57">
-        <v>0.6939309985236987</v>
+        <v>0.6917277029549935</v>
       </c>
       <c r="K57">
-        <v>1.291610433615147</v>
+        <v>0.9806152097354205</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -2582,10 +2582,10 @@
         <v>-1.396925731356437</v>
       </c>
       <c r="J58">
-        <v>4.389641941562725</v>
+        <v>4.418359273719397</v>
       </c>
       <c r="K58">
-        <v>0.9421454668186237</v>
+        <v>0.3116592438309069</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -2620,10 +2620,10 @@
         <v>7.248005045717345</v>
       </c>
       <c r="J59">
-        <v>-2.897775518196724</v>
+        <v>-2.918358060209926</v>
       </c>
       <c r="K59">
-        <v>2.376675949702928</v>
+        <v>2.165209903589496</v>
       </c>
       <c r="L59">
         <v>1</v>
@@ -2658,10 +2658,10 @@
         <v>1.595539792285734</v>
       </c>
       <c r="J60">
-        <v>3.536599664816866</v>
+        <v>3.545631968633211</v>
       </c>
       <c r="K60">
-        <v>0.6913306360780416</v>
+        <v>0.4554643854324951</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -2696,10 +2696,10 @@
         <v>-1.108832386547995</v>
       </c>
       <c r="J61">
-        <v>4.081433151074503</v>
+        <v>4.068905471202674</v>
       </c>
       <c r="K61">
-        <v>1.029991063312985</v>
+        <v>0.9304965358973398</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -2734,10 +2734,10 @@
         <v>-1.375544769494584</v>
       </c>
       <c r="J62">
-        <v>1.113154461572001</v>
+        <v>1.085125334189059</v>
       </c>
       <c r="K62">
-        <v>0.3169775007859106</v>
+        <v>0.6462348536669827</v>
       </c>
       <c r="L62">
         <v>0</v>
@@ -2772,10 +2772,10 @@
         <v>-0.5168061034656545</v>
       </c>
       <c r="J63">
-        <v>4.131522281054397</v>
+        <v>4.133386136384054</v>
       </c>
       <c r="K63">
-        <v>0.4910989400142807</v>
+        <v>0.309669683287446</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -2810,10 +2810,10 @@
         <v>-1.696653016625957</v>
       </c>
       <c r="J64">
-        <v>2.674654472356502</v>
+        <v>2.647122749020131</v>
       </c>
       <c r="K64">
-        <v>2.259459449904067</v>
+        <v>2.122963236514359</v>
       </c>
       <c r="L64">
         <v>1</v>
@@ -2848,10 +2848,10 @@
         <v>1.328617033126034</v>
       </c>
       <c r="J65">
-        <v>3.580444366231029</v>
+        <v>3.585590995043632</v>
       </c>
       <c r="K65">
-        <v>1.326903352322395</v>
+        <v>0.9252861000559829</v>
       </c>
       <c r="L65">
         <v>0</v>
@@ -2886,10 +2886,10 @@
         <v>3.885391830535232</v>
       </c>
       <c r="J66">
-        <v>2.697133528728628</v>
+        <v>2.704240897284671</v>
       </c>
       <c r="K66">
-        <v>-0.4341001766086149</v>
+        <v>-0.52684841405158</v>
       </c>
       <c r="L66">
         <v>0</v>
@@ -2924,10 +2924,10 @@
         <v>-2.051427681756635</v>
       </c>
       <c r="J67">
-        <v>-1.017530713072893</v>
+        <v>-0.9665085356969599</v>
       </c>
       <c r="K67">
-        <v>-0.5994438997386343</v>
+        <v>-1.405996776207781</v>
       </c>
       <c r="L67">
         <v>0</v>
@@ -2962,10 +2962,10 @@
         <v>-1.389208558780749</v>
       </c>
       <c r="J68">
-        <v>-0.3132090150668209</v>
+        <v>-0.2596148689668182</v>
       </c>
       <c r="K68">
-        <v>-0.7672438687289876</v>
+        <v>-1.548481718498014</v>
       </c>
       <c r="L68">
         <v>0</v>
@@ -3000,10 +3000,10 @@
         <v>3.195217519734896</v>
       </c>
       <c r="J69">
-        <v>-1.438560990583636</v>
+        <v>-1.414429167061006</v>
       </c>
       <c r="K69">
-        <v>-0.2498009530101797</v>
+        <v>-0.4347266286248254</v>
       </c>
       <c r="L69">
         <v>1</v>
@@ -3038,10 +3038,10 @@
         <v>-0.9920165335750283</v>
       </c>
       <c r="J70">
-        <v>0.2326554497465709</v>
+        <v>0.2707647368076531</v>
       </c>
       <c r="K70">
-        <v>-0.5793069632780093</v>
+        <v>-0.9916517804791293</v>
       </c>
       <c r="L70">
         <v>0</v>
@@ -3076,10 +3076,10 @@
         <v>-3.876174042005317</v>
       </c>
       <c r="J71">
-        <v>-0.8047384482836779</v>
+        <v>-0.7691302958146836</v>
       </c>
       <c r="K71">
-        <v>-0.9751867463888328</v>
+        <v>-1.2936049343673</v>
       </c>
       <c r="L71">
         <v>0</v>
@@ -3114,10 +3114,10 @@
         <v>-1.490705917576324</v>
       </c>
       <c r="J72">
-        <v>-1.420307271366104</v>
+        <v>-1.397289040705116</v>
       </c>
       <c r="K72">
-        <v>-0.0298920967535687</v>
+        <v>-0.2933279077840871</v>
       </c>
       <c r="L72">
         <v>1</v>
@@ -3152,10 +3152,10 @@
         <v>7.402037509448133</v>
       </c>
       <c r="J73">
-        <v>-1.406692857238542</v>
+        <v>-1.357435171118281</v>
       </c>
       <c r="K73">
-        <v>-0.008676943915843321</v>
+        <v>-0.8498617890073193</v>
       </c>
       <c r="L73">
         <v>0</v>
@@ -3190,10 +3190,10 @@
         <v>2.04979063311115</v>
       </c>
       <c r="J74">
-        <v>-0.4212937892735217</v>
+        <v>-0.3648179102591159</v>
       </c>
       <c r="K74">
-        <v>-1.53079279837333</v>
+        <v>-2.069057061871924</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -3228,10 +3228,10 @@
         <v>-1.63859163868917</v>
       </c>
       <c r="J75">
-        <v>-2.981606906976433</v>
+        <v>-3.013784938439342</v>
       </c>
       <c r="K75">
-        <v>0.1936897238049635</v>
+        <v>0.7403713672876893</v>
       </c>
       <c r="L75">
         <v>1</v>
@@ -3266,10 +3266,10 @@
         <v>2.701193626844962</v>
       </c>
       <c r="J76">
-        <v>-2.119328960839848</v>
+        <v>-2.156112636127928</v>
       </c>
       <c r="K76">
-        <v>3.307773830859092</v>
+        <v>2.954834589545165</v>
       </c>
       <c r="L76">
         <v>1</v>
@@ -3304,10 +3304,10 @@
         <v>1.22697560004966</v>
       </c>
       <c r="J77">
-        <v>-0.141825183420899</v>
+        <v>-0.1306690773264085</v>
       </c>
       <c r="K77">
-        <v>-1.525288131158192</v>
+        <v>-1.062800669431207</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -3342,10 +3342,10 @@
         <v>-2.748043546880432</v>
       </c>
       <c r="J78">
-        <v>-1.628644432134937</v>
+        <v>-1.656584375609297</v>
       </c>
       <c r="K78">
-        <v>0.4276927757187874</v>
+        <v>0.5759334384023763</v>
       </c>
       <c r="L78">
         <v>1</v>
@@ -3380,10 +3380,10 @@
         <v>1.438500149618355</v>
       </c>
       <c r="J79">
-        <v>-1.456659934391126</v>
+        <v>-1.519340912291312</v>
       </c>
       <c r="K79">
-        <v>1.404397231512907</v>
+        <v>2.136679113478325</v>
       </c>
       <c r="L79">
         <v>1</v>
@@ -3418,10 +3418,10 @@
         <v>-1.851309254365192</v>
       </c>
       <c r="J80">
-        <v>-2.007192359781172</v>
+        <v>-2.012610873880127</v>
       </c>
       <c r="K80">
-        <v>-0.2355986197722643</v>
+        <v>0.04906338939520065</v>
       </c>
       <c r="L80">
         <v>1</v>
@@ -3456,10 +3456,10 @@
         <v>1.601042232620718</v>
       </c>
       <c r="J81">
-        <v>-2.36701406803588</v>
+        <v>-2.373814829667429</v>
       </c>
       <c r="K81">
-        <v>1.008242865411149</v>
+        <v>0.7488063939766041</v>
       </c>
       <c r="L81">
         <v>1</v>
@@ -3494,10 +3494,10 @@
         <v>-3.047763421334094</v>
       </c>
       <c r="J82">
-        <v>-2.135994739583369</v>
+        <v>-2.196308041708005</v>
       </c>
       <c r="K82">
-        <v>4.835303277017405</v>
+        <v>4.573101935022289</v>
       </c>
       <c r="L82">
         <v>1</v>
@@ -3532,10 +3532,10 @@
         <v>-0.2421797588662415</v>
       </c>
       <c r="J83">
-        <v>-2.409818117552785</v>
+        <v>-2.466694098429016</v>
       </c>
       <c r="K83">
-        <v>0.7627791445385282</v>
+        <v>1.516788047154356</v>
       </c>
       <c r="L83">
         <v>1</v>
@@ -3570,10 +3570,10 @@
         <v>-0.3292851436271967</v>
       </c>
       <c r="J84">
-        <v>-0.720260457492957</v>
+        <v>-0.7387530716443518</v>
       </c>
       <c r="K84">
-        <v>-0.6658829209057285</v>
+        <v>-0.1875852085284164</v>
       </c>
       <c r="L84">
         <v>1</v>
@@ -3608,10 +3608,10 @@
         <v>-2.171446569789886</v>
       </c>
       <c r="J85">
-        <v>-0.8488760041571299</v>
+        <v>-0.8875331942129598</v>
       </c>
       <c r="K85">
-        <v>1.873498021372845</v>
+        <v>2.015604111375967</v>
       </c>
       <c r="L85">
         <v>1</v>
@@ -3646,10 +3646,10 @@
         <v>-1.395634443405399</v>
       </c>
       <c r="J86">
-        <v>2.682139358693337</v>
+        <v>2.621215496246246</v>
       </c>
       <c r="K86">
-        <v>3.407870326944026</v>
+        <v>3.446844403842952</v>
       </c>
       <c r="L86">
         <v>0</v>
@@ -3684,10 +3684,10 @@
         <v>2.88149177501296</v>
       </c>
       <c r="J87">
-        <v>-1.246775895669333</v>
+        <v>-1.271921292889235</v>
       </c>
       <c r="K87">
-        <v>-0.250339156046635</v>
+        <v>0.2628798037917416</v>
       </c>
       <c r="L87">
         <v>1</v>
@@ -3722,10 +3722,10 @@
         <v>-4.027374994008608</v>
       </c>
       <c r="J88">
-        <v>0.7731082905873745</v>
+        <v>0.7705782996493188</v>
       </c>
       <c r="K88">
-        <v>0.2134639871487606</v>
+        <v>0.208210010538873</v>
       </c>
       <c r="L88">
         <v>1</v>
@@ -3760,10 +3760,10 @@
         <v>0.5188096463582872</v>
       </c>
       <c r="J89">
-        <v>-1.882034091761978</v>
+        <v>-1.873740537590707</v>
       </c>
       <c r="K89">
-        <v>-0.1560734441784014</v>
+        <v>-0.374406614514349</v>
       </c>
       <c r="L89">
         <v>1</v>
@@ -3798,10 +3798,10 @@
         <v>1.676868261170144</v>
       </c>
       <c r="J90">
-        <v>-2.757219139561503</v>
+        <v>-2.74453667142197</v>
       </c>
       <c r="K90">
-        <v>-0.01651475817854805</v>
+        <v>-0.6094534483163685</v>
       </c>
       <c r="L90">
         <v>0</v>
@@ -3836,10 +3836,10 @@
         <v>0.7468536645065109</v>
       </c>
       <c r="J91">
-        <v>-1.62913740524205</v>
+        <v>-1.620632978964677</v>
       </c>
       <c r="K91">
-        <v>-0.2154189447183144</v>
+        <v>-0.435258230979105</v>
       </c>
       <c r="L91">
         <v>1</v>
@@ -3874,10 +3874,10 @@
         <v>2.649400308885781</v>
       </c>
       <c r="J92">
-        <v>-1.142637686414687</v>
+        <v>-1.138227112571925</v>
       </c>
       <c r="K92">
-        <v>0.4000315849688777</v>
+        <v>-0.002338189601958308</v>
       </c>
       <c r="L92">
         <v>0</v>
@@ -3912,10 +3912,10 @@
         <v>-0.5661498033962505</v>
       </c>
       <c r="J93">
-        <v>-3.697824501182436</v>
+        <v>-3.767742693443275</v>
       </c>
       <c r="K93">
-        <v>1.924492558882939</v>
+        <v>2.437789613452201</v>
       </c>
       <c r="L93">
         <v>1</v>
@@ -3950,10 +3950,10 @@
         <v>0.9022839838509789</v>
       </c>
       <c r="J94">
-        <v>-1.557244719264894</v>
+        <v>-1.523397682987389</v>
       </c>
       <c r="K94">
-        <v>0.1260408928672117</v>
+        <v>-0.5445105571779282</v>
       </c>
       <c r="L94">
         <v>1</v>
@@ -3988,10 +3988,10 @@
         <v>1.095279105472553</v>
       </c>
       <c r="J95">
-        <v>-3.732670272037806</v>
+        <v>-3.712355209355719</v>
       </c>
       <c r="K95">
-        <v>1.487296881576583</v>
+        <v>0.5832085602830784</v>
       </c>
       <c r="L95">
         <v>1</v>
@@ -4026,10 +4026,10 @@
         <v>3.48180375592971</v>
       </c>
       <c r="J96">
-        <v>-3.631678089825821</v>
+        <v>-3.589471834049838</v>
       </c>
       <c r="K96">
-        <v>0.2646755379076824</v>
+        <v>-0.6509914030748747</v>
       </c>
       <c r="L96">
         <v>1</v>
@@ -4064,10 +4064,10 @@
         <v>3.42933179280484</v>
       </c>
       <c r="J97">
-        <v>-0.9151596539522665</v>
+        <v>-0.8746099639171652</v>
       </c>
       <c r="K97">
-        <v>0.1679730231007844</v>
+        <v>-0.4676504245114074</v>
       </c>
       <c r="L97">
         <v>0</v>
@@ -4102,10 +4102,10 @@
         <v>0.5146236897519318</v>
       </c>
       <c r="J98">
-        <v>-0.5550887198972978</v>
+        <v>-0.5581053148647364</v>
       </c>
       <c r="K98">
-        <v>-0.10339726750294</v>
+        <v>0.05071800932898181</v>
       </c>
       <c r="L98">
         <v>1</v>
@@ -4140,10 +4140,10 @@
         <v>-3.446059161832602</v>
       </c>
       <c r="J99">
-        <v>-3.273559853763337</v>
+        <v>-3.357810168343565</v>
       </c>
       <c r="K99">
-        <v>1.963776109686695</v>
+        <v>2.631267345205423</v>
       </c>
       <c r="L99">
         <v>1</v>
@@ -4178,10 +4178,10 @@
         <v>-2.3683053675189</v>
       </c>
       <c r="J100">
-        <v>0.9083368976162672</v>
+        <v>0.8596398349399202</v>
       </c>
       <c r="K100">
-        <v>1.780725145839351</v>
+        <v>2.222372981547321</v>
       </c>
       <c r="L100">
         <v>1</v>
@@ -4216,10 +4216,10 @@
         <v>9.227053871596571</v>
       </c>
       <c r="J101">
-        <v>-0.7604361484473698</v>
+        <v>-0.77473496795699</v>
       </c>
       <c r="K101">
-        <v>1.019133983609076</v>
+        <v>1.12149230855876</v>
       </c>
       <c r="L101">
         <v>1</v>
@@ -4254,10 +4254,10 @@
         <v>7.48842988375196</v>
       </c>
       <c r="J102">
-        <v>0.1324753265098149</v>
+        <v>0.09333794598401499</v>
       </c>
       <c r="K102">
-        <v>1.000071938479992</v>
+        <v>1.470654506350435</v>
       </c>
       <c r="L102">
         <v>1</v>
@@ -4292,10 +4292,10 @@
         <v>3.461479188801734</v>
       </c>
       <c r="J103">
-        <v>0.2096014835043384</v>
+        <v>0.2036495632861241</v>
       </c>
       <c r="K103">
-        <v>-0.4988436782447908</v>
+        <v>-0.2316999632625758</v>
       </c>
       <c r="L103">
         <v>1</v>
@@ -4330,10 +4330,10 @@
         <v>2.68555476004972</v>
       </c>
       <c r="J104">
-        <v>-0.835913541259185</v>
+        <v>-0.8308085811033362</v>
       </c>
       <c r="K104">
-        <v>-0.5553420096006298</v>
+        <v>-0.4661426743499366</v>
       </c>
       <c r="L104">
         <v>1</v>
@@ -4368,10 +4368,10 @@
         <v>-1.265586690638589</v>
       </c>
       <c r="J105">
-        <v>-0.9155844788534524</v>
+        <v>-0.9523207895078756</v>
       </c>
       <c r="K105">
-        <v>-0.2649006362459438</v>
+        <v>0.3418601678584471</v>
       </c>
       <c r="L105">
         <v>0</v>
@@ -4406,10 +4406,10 @@
         <v>-1.31706712820111</v>
       </c>
       <c r="J106">
-        <v>-0.332163480509168</v>
+        <v>-0.3420103838707607</v>
       </c>
       <c r="K106">
-        <v>-1.359300074160894</v>
+        <v>-0.987785698919368</v>
       </c>
       <c r="L106">
         <v>0</v>
@@ -4444,10 +4444,10 @@
         <v>-2.373498775940256</v>
       </c>
       <c r="J107">
-        <v>0.2888512846061017</v>
+        <v>0.2861492414350866</v>
       </c>
       <c r="K107">
-        <v>0.6022358284919079</v>
+        <v>0.572353750214518</v>
       </c>
       <c r="L107">
         <v>1</v>
@@ -4482,10 +4482,10 @@
         <v>-3.668547366861195</v>
       </c>
       <c r="J108">
-        <v>2.5445993253794</v>
+        <v>2.568016147926743</v>
       </c>
       <c r="K108">
-        <v>-2.72112936096038</v>
+        <v>-2.49370255281813</v>
       </c>
       <c r="L108">
         <v>0</v>
@@ -4520,10 +4520,10 @@
         <v>-5.791285481056422</v>
       </c>
       <c r="J109">
-        <v>-0.450527964421376</v>
+        <v>-0.4323397627312239</v>
       </c>
       <c r="K109">
-        <v>-1.521039226026822</v>
+        <v>-1.72588637437161</v>
       </c>
       <c r="L109">
         <v>0</v>
@@ -4558,10 +4558,10 @@
         <v>-1.139896679783599</v>
       </c>
       <c r="J110">
-        <v>-1.062415540041625</v>
+        <v>-1.071934182405653</v>
       </c>
       <c r="K110">
-        <v>-1.474114404985998</v>
+        <v>-1.078896508776524</v>
       </c>
       <c r="L110">
         <v>1</v>
@@ -4596,10 +4596,10 @@
         <v>-4.351709897196057</v>
       </c>
       <c r="J111">
-        <v>-1.082866487320272</v>
+        <v>-1.081024754240615</v>
       </c>
       <c r="K111">
-        <v>-0.2902077308435257</v>
+        <v>-0.2384073729823436</v>
       </c>
       <c r="L111">
         <v>0</v>
@@ -4634,10 +4634,10 @@
         <v>0.9352901544665151</v>
       </c>
       <c r="J112">
-        <v>-0.3855884763463622</v>
+        <v>-0.3913546956058774</v>
       </c>
       <c r="K112">
-        <v>-1.656917169351016</v>
+        <v>-1.188998212174408</v>
       </c>
       <c r="L112">
         <v>0</v>
@@ -4672,10 +4672,10 @@
         <v>1.798898625013951</v>
       </c>
       <c r="J113">
-        <v>-0.1520130997941832</v>
+        <v>-0.135493283977983</v>
       </c>
       <c r="K113">
-        <v>-0.9242864264995382</v>
+        <v>-0.8872761707372598</v>
       </c>
       <c r="L113">
         <v>0</v>
@@ -4710,10 +4710,10 @@
         <v>4.770798957649014</v>
       </c>
       <c r="J114">
-        <v>-1.387399040961992</v>
+        <v>-1.377994135518526</v>
       </c>
       <c r="K114">
-        <v>-1.151699170626322</v>
+        <v>-1.061724087911554</v>
       </c>
       <c r="L114">
         <v>1</v>
@@ -4748,10 +4748,10 @@
         <v>-3.445681157825471</v>
       </c>
       <c r="J115">
-        <v>-1.335541592301181</v>
+        <v>-1.318540757348595</v>
       </c>
       <c r="K115">
-        <v>-1.45935264329937</v>
+        <v>-1.498881582341291</v>
       </c>
       <c r="L115">
         <v>0</v>
@@ -4786,10 +4786,10 @@
         <v>-2.375444732249699</v>
       </c>
       <c r="J116">
-        <v>-0.07831823193758869</v>
+        <v>-0.1326264405081925</v>
       </c>
       <c r="K116">
-        <v>0.6250001523181354</v>
+        <v>1.437952833379338</v>
       </c>
       <c r="L116">
         <v>0</v>
@@ -4824,10 +4824,10 @@
         <v>-2.589819457791724</v>
       </c>
       <c r="J117">
-        <v>0.2229671683770243</v>
+        <v>0.1609165356732134</v>
       </c>
       <c r="K117">
-        <v>0.4942374856972773</v>
+        <v>1.345610820585496</v>
       </c>
       <c r="L117">
         <v>0</v>
@@ -4862,10 +4862,10 @@
         <v>-0.2857214052294005</v>
       </c>
       <c r="J118">
-        <v>-0.9406878917459208</v>
+        <v>-0.9882906728122068</v>
       </c>
       <c r="K118">
-        <v>0.5196334450229927</v>
+        <v>1.159776873653835</v>
       </c>
       <c r="L118">
         <v>0</v>
@@ -4900,10 +4900,10 @@
         <v>1.786101357636882</v>
       </c>
       <c r="J119">
-        <v>1.966279918837412</v>
+        <v>1.985961104028641</v>
       </c>
       <c r="K119">
-        <v>-2.704530549632327</v>
+        <v>-2.320520479605298</v>
       </c>
       <c r="L119">
         <v>0</v>
@@ -4938,10 +4938,10 @@
         <v>3.021039694056401</v>
       </c>
       <c r="J120">
-        <v>0.4371437440427725</v>
+        <v>0.4357448884218485</v>
       </c>
       <c r="K120">
-        <v>-1.364565835283597</v>
+        <v>-1.1057443757332</v>
       </c>
       <c r="L120">
         <v>0</v>
@@ -4976,10 +4976,10 @@
         <v>-2.304091133233749</v>
       </c>
       <c r="J121">
-        <v>1.1343428881678</v>
+        <v>1.121149362837934</v>
       </c>
       <c r="K121">
-        <v>-0.2329460890681233</v>
+        <v>0.04637045257509789</v>
       </c>
       <c r="L121">
         <v>0</v>
@@ -5014,10 +5014,10 @@
         <v>-1.872823404746111</v>
       </c>
       <c r="J122">
-        <v>-2.453204887180899</v>
+        <v>-2.446176424434344</v>
       </c>
       <c r="K122">
-        <v>-0.3795952447119978</v>
+        <v>-0.553172024579344</v>
       </c>
       <c r="L122">
         <v>1</v>
@@ -5052,10 +5052,10 @@
         <v>-1.774049697659439</v>
       </c>
       <c r="J123">
-        <v>0.6626056346635369</v>
+        <v>0.7078458966038875</v>
       </c>
       <c r="K123">
-        <v>-2.344622199985934</v>
+        <v>-2.401446438444018</v>
       </c>
       <c r="L123">
         <v>0</v>
@@ -5090,10 +5090,10 @@
         <v>-3.632124300685543</v>
       </c>
       <c r="J124">
-        <v>3.53582034342602</v>
+        <v>3.544434936902069</v>
       </c>
       <c r="K124">
-        <v>-0.8829712230890328</v>
+        <v>-0.8704557115281998</v>
       </c>
       <c r="L124">
         <v>0</v>
@@ -5128,10 +5128,10 @@
         <v>3.453900764972414</v>
       </c>
       <c r="J125">
-        <v>-0.2738543662988833</v>
+        <v>-0.2671078815878193</v>
       </c>
       <c r="K125">
-        <v>0.8355271527903523</v>
+        <v>0.3038783761588723</v>
       </c>
       <c r="L125">
         <v>0</v>
@@ -5166,10 +5166,10 @@
         <v>-1.324016105236785</v>
       </c>
       <c r="J126">
-        <v>-1.027719006777317</v>
+        <v>-1.033891792412623</v>
       </c>
       <c r="K126">
-        <v>0.6433035822991269</v>
+        <v>0.7013003942886813</v>
       </c>
       <c r="L126">
         <v>0</v>
@@ -5204,10 +5204,10 @@
         <v>2.379768236500968</v>
       </c>
       <c r="J127">
-        <v>-1.848021448478303</v>
+        <v>-1.920185595372564</v>
       </c>
       <c r="K127">
-        <v>2.255835669071952</v>
+        <v>2.968714461516309</v>
       </c>
       <c r="L127">
         <v>1</v>
@@ -5242,10 +5242,10 @@
         <v>-2.648737625958293</v>
       </c>
       <c r="J128">
-        <v>-0.6150069677244498</v>
+        <v>-0.6385931942795091</v>
       </c>
       <c r="K128">
-        <v>-0.3393282439151568</v>
+        <v>0.2260094278718011</v>
       </c>
       <c r="L128">
         <v>0</v>
@@ -5280,10 +5280,10 @@
         <v>0.6581962167362199</v>
       </c>
       <c r="J129">
-        <v>-0.6187479542484274</v>
+        <v>-0.5749032238970893</v>
       </c>
       <c r="K129">
-        <v>-0.5034464118218474</v>
+        <v>-1.174312723778609</v>
       </c>
       <c r="L129">
         <v>0</v>
@@ -5318,10 +5318,10 @@
         <v>-2.358321197761798</v>
       </c>
       <c r="J130">
-        <v>-2.217688418011824</v>
+        <v>-2.279247473057755</v>
       </c>
       <c r="K130">
-        <v>0.5400016238660555</v>
+        <v>1.207279679882197</v>
       </c>
       <c r="L130">
         <v>1</v>
@@ -5356,10 +5356,10 @@
         <v>4.535346417536212</v>
       </c>
       <c r="J131">
-        <v>0.137064802943281</v>
+        <v>0.1343554839672817</v>
       </c>
       <c r="K131">
-        <v>0.7556291150031117</v>
+        <v>0.6501664089785053</v>
       </c>
       <c r="L131">
         <v>0</v>
@@ -5394,10 +5394,10 @@
         <v>-1.500344054375704</v>
       </c>
       <c r="J132">
-        <v>2.962114816421304</v>
+        <v>2.984981318581569</v>
       </c>
       <c r="K132">
-        <v>0.9459886990146188</v>
+        <v>0.36776541095631</v>
       </c>
       <c r="L132">
         <v>0</v>
@@ -5432,10 +5432,10 @@
         <v>-2.743586783491561</v>
       </c>
       <c r="J133">
-        <v>-0.9527221965969082</v>
+        <v>-0.9552055800040427</v>
       </c>
       <c r="K133">
-        <v>0.2545198186505009</v>
+        <v>0.213327401821901</v>
       </c>
       <c r="L133">
         <v>0</v>
@@ -5470,10 +5470,10 @@
         <v>6.500858816274786</v>
       </c>
       <c r="J134">
-        <v>-1.726281044344406</v>
+        <v>-1.728489247816013</v>
       </c>
       <c r="K134">
-        <v>0.3457428096510733</v>
+        <v>0.2490280651440062</v>
       </c>
       <c r="L134">
         <v>1</v>
@@ -5508,10 +5508,10 @@
         <v>-1.987819018762579</v>
       </c>
       <c r="J135">
-        <v>-1.022679760791386</v>
+        <v>-1.016568627843067</v>
       </c>
       <c r="K135">
-        <v>-1.234910428562822</v>
+        <v>-1.022689439960918</v>
       </c>
       <c r="L135">
         <v>0</v>
@@ -5546,10 +5546,10 @@
         <v>0.02181115967541872</v>
       </c>
       <c r="J136">
-        <v>1.76038150877923</v>
+        <v>1.715377368062478</v>
       </c>
       <c r="K136">
-        <v>-0.006628744333474798</v>
+        <v>0.5186499182702348</v>
       </c>
       <c r="L136">
         <v>0</v>
@@ -5584,10 +5584,10 @@
         <v>-4.512653359680607</v>
       </c>
       <c r="J137">
-        <v>-0.2331305328650757</v>
+        <v>-0.22796728079162</v>
       </c>
       <c r="K137">
-        <v>-1.176109359872265</v>
+        <v>-0.8357031671616798</v>
       </c>
       <c r="L137">
         <v>0</v>
@@ -5622,10 +5622,10 @@
         <v>-2.432049741316328</v>
       </c>
       <c r="J138">
-        <v>-2.015435156365597</v>
+        <v>-2.029912792884849</v>
       </c>
       <c r="K138">
-        <v>-0.2167569529930961</v>
+        <v>0.1042433177769808</v>
       </c>
       <c r="L138">
         <v>1</v>
@@ -5660,10 +5660,10 @@
         <v>-1.393410939443583</v>
       </c>
       <c r="J139">
-        <v>-1.315316276251979</v>
+        <v>-1.293404701632331</v>
       </c>
       <c r="K139">
-        <v>-1.117285175713702</v>
+        <v>-1.132094979379374</v>
       </c>
       <c r="L139">
         <v>0</v>
@@ -5698,10 +5698,10 @@
         <v>-1.231508195208441</v>
       </c>
       <c r="J140">
-        <v>-2.120035644323627</v>
+        <v>-2.111265469491915</v>
       </c>
       <c r="K140">
-        <v>-0.6052211220723906</v>
+        <v>-0.7343623395973875</v>
       </c>
       <c r="L140">
         <v>1</v>
@@ -5736,10 +5736,10 @@
         <v>-4.336959714438739</v>
       </c>
       <c r="J141">
-        <v>-1.792122567793316</v>
+        <v>-1.797163680840558</v>
       </c>
       <c r="K141">
-        <v>0.3225840297751258</v>
+        <v>0.4364608083889347</v>
       </c>
       <c r="L141">
         <v>1</v>
@@ -5774,10 +5774,10 @@
         <v>6.105986216995588</v>
       </c>
       <c r="J142">
-        <v>0.2136280429757419</v>
+        <v>0.2304982161531181</v>
       </c>
       <c r="K142">
-        <v>-0.3266758966449397</v>
+        <v>-0.3842241327485074</v>
       </c>
       <c r="L142">
         <v>0</v>
@@ -5812,10 +5812,10 @@
         <v>-2.159502993277289</v>
       </c>
       <c r="J143">
-        <v>1.729683970102134</v>
+        <v>1.782774293480688</v>
       </c>
       <c r="K143">
-        <v>0.9805739616141812</v>
+        <v>0.08954385542560585</v>
       </c>
       <c r="L143">
         <v>0</v>
@@ -5850,10 +5850,10 @@
         <v>4.255087865448534</v>
       </c>
       <c r="J144">
-        <v>-0.4517499657218387</v>
+        <v>-0.417645917060643</v>
       </c>
       <c r="K144">
-        <v>1.046355692036821</v>
+        <v>0.3685675565701083</v>
       </c>
       <c r="L144">
         <v>0</v>
@@ -5888,10 +5888,10 @@
         <v>0.9764638399541132</v>
       </c>
       <c r="J145">
-        <v>0.8752581790224195</v>
+        <v>0.8433658609412374</v>
       </c>
       <c r="K145">
-        <v>-1.430631163059595</v>
+        <v>-0.3337359934514366</v>
       </c>
       <c r="L145">
         <v>0</v>

</xml_diff>